<commit_message>
Import Sales Lines from Excel
</commit_message>
<xml_diff>
--- a/Excel Import - Copy.xlsx
+++ b/Excel Import - Copy.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AL\InternTasks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\AL\InternTaskDocker\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0601144B-C15D-40FF-BCD4-E799F0B4B127}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BC3502E-B677-4E9C-893A-C11E4CD5D021}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1560" yWindow="1560" windowWidth="22245" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1710" yWindow="1380" windowWidth="18975" windowHeight="13185" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Items" sheetId="1" r:id="rId1"/>
@@ -445,7 +445,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -507,9 +507,6 @@
       <c r="D3" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="E3">
-        <v>150.30000000000001</v>
-      </c>
       <c r="F3" s="2" t="s">
         <v>12</v>
       </c>

</xml_diff>